<commit_message>
AV3 Arq. Comput 20Jun2023
</commit_message>
<xml_diff>
--- a/03 Assessments/Perdeu 1 aluno AV2 1001 - Arq de Computadores 2023.1(1-36).xlsx
+++ b/03 Assessments/Perdeu 1 aluno AV2 1001 - Arq de Computadores 2023.1(1-36).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\22 WydenArea1ArquiteturaComputadores\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A8944B-8779-4221-BB5D-2FD2D2355C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0092D4-9747-4A95-BB72-E6F9F140E945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="153">
   <si>
     <t>ID</t>
   </si>
@@ -535,6 +535,9 @@
   </si>
   <si>
     <t>diminuição da fragmentação.</t>
+  </si>
+  <si>
+    <t>Atualizado p/4,8 - atividades</t>
   </si>
 </sst>
 </file>
@@ -542,9 +545,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,13 +555,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -573,10 +598,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,7 +719,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -706,10 +734,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1083,7 +1111,7 @@
   <dimension ref="A1:AR37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,7 +1771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10</v>
       </c>
@@ -1756,13 +1784,16 @@
       <c r="D8" t="s">
         <v>44</v>
       </c>
-      <c r="F8">
+      <c r="E8" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F8" s="5">
         <v>4</v>
       </c>
       <c r="H8" s="1">
         <v>45080.431851851798</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="3" t="s">
         <v>80</v>
       </c>
       <c r="L8" s="2" t="s">

</xml_diff>